<commit_message>
docs: readme, api docs, scrum docs etc.
</commit_message>
<xml_diff>
--- a/documents/API명세서.xlsx
+++ b/documents/API명세서.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\numble\CrySeller\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE10527-3F48-42A3-80C7-18D1F8D55318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6F6CFE-3F32-48A9-9094-32419004EDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="2715" windowWidth="22875" windowHeight="12150" xr2:uid="{6B7D753C-8BB7-45EF-993C-18B14307E70B}"/>
+    <workbookView xWindow="1668" yWindow="0" windowWidth="15288" windowHeight="12360" xr2:uid="{6B7D753C-8BB7-45EF-993C-18B14307E70B}"/>
   </bookViews>
   <sheets>
     <sheet name="API Documentation" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,10 +210,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/users/withdrawl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/users</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,6 +247,42 @@
   </si>
   <si>
     <t>PathVariable(item_no), RequestBody(item_info...)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/categories</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;Category&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리목록조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리상세조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/categories/{no}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PathVariable(category_no)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/users/withdrawal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -621,22 +653,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF574D46-F872-4793-A475-11A390D27F91}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -707,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -734,7 +766,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
@@ -758,7 +790,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -785,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -814,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -838,13 +870,13 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -862,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -886,7 +918,7 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
@@ -910,7 +942,7 @@
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
         <v>21</v>
@@ -936,7 +968,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
         <v>21</v>
@@ -948,10 +980,61 @@
         <v>22</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>